<commit_message>
fig S4-6 and supp tables
</commit_message>
<xml_diff>
--- a/results/supplement/tables/Table_S2.xlsx
+++ b/results/supplement/tables/Table_S2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metatranscriptomes (cDNA)" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Raw reads pairs</t>
     </r>
@@ -43,6 +44,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -54,6 +56,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Quality trimmed</t>
     </r>
@@ -64,6 +67,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -75,6 +79,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mapped to Assembly</t>
     </r>
@@ -85,6 +90,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -95,6 +101,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Streptomycin – </t>
     </r>
@@ -104,6 +111,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C. difficile</t>
     </r>
@@ -112,6 +120,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> infected</t>
     </r>
@@ -125,6 +134,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cefoperazone – </t>
     </r>
@@ -134,6 +144,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C. difficile</t>
     </r>
@@ -142,6 +153,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> infected</t>
     </r>
@@ -155,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Clindamycin – </t>
     </r>
@@ -164,6 +177,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">C. difficile</t>
     </r>
@@ -172,6 +186,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> infected</t>
     </r>
@@ -210,6 +225,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -231,6 +247,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -238,12 +255,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,17 +335,17 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,17 +435,17 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,7 +520,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -522,12 +541,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>